<commit_message>
update lagi 6 juni
</commit_message>
<xml_diff>
--- a/Y_pred.xlsx
+++ b/Y_pred.xlsx
@@ -930,7 +930,7 @@
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101">
@@ -2575,7 +2575,7 @@
     </row>
     <row r="429">
       <c r="A429" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="430">
@@ -5010,7 +5010,7 @@
     </row>
     <row r="916">
       <c r="A916" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="917">
@@ -5815,7 +5815,7 @@
     </row>
     <row r="1077">
       <c r="A1077" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1078">
@@ -5960,7 +5960,7 @@
     </row>
     <row r="1106">
       <c r="A1106" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1107">
@@ -6020,7 +6020,7 @@
     </row>
     <row r="1118">
       <c r="A1118" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1119">
@@ -6105,7 +6105,7 @@
     </row>
     <row r="1135">
       <c r="A1135" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1136">
@@ -7210,7 +7210,7 @@
     </row>
     <row r="1356">
       <c r="A1356" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1357">
@@ -9490,7 +9490,7 @@
     </row>
     <row r="1812">
       <c r="A1812" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1813">
@@ -9980,7 +9980,7 @@
     </row>
     <row r="1910">
       <c r="A1910" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1911">
@@ -12150,7 +12150,7 @@
     </row>
     <row r="2344">
       <c r="A2344" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2345">
@@ -12515,7 +12515,7 @@
     </row>
     <row r="2417">
       <c r="A2417" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2418">
@@ -14545,7 +14545,7 @@
     </row>
     <row r="2823">
       <c r="A2823" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2824">
@@ -16355,7 +16355,7 @@
     </row>
     <row r="3185">
       <c r="A3185" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3186">
@@ -18235,7 +18235,7 @@
     </row>
     <row r="3561">
       <c r="A3561" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3562">
@@ -18510,7 +18510,7 @@
     </row>
     <row r="3616">
       <c r="A3616" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3617">
@@ -18850,7 +18850,7 @@
     </row>
     <row r="3684">
       <c r="A3684" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3685">
@@ -20075,7 +20075,7 @@
     </row>
     <row r="3929">
       <c r="A3929" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3930">
@@ -22330,7 +22330,7 @@
     </row>
     <row r="4380">
       <c r="A4380" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4381">
@@ -22865,7 +22865,7 @@
     </row>
     <row r="4487">
       <c r="A4487" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4488">
@@ -24555,7 +24555,7 @@
     </row>
     <row r="4825">
       <c r="A4825" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4826">
@@ -26320,7 +26320,7 @@
     </row>
     <row r="5178">
       <c r="A5178" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5179">
@@ -27330,7 +27330,7 @@
     </row>
     <row r="5380">
       <c r="A5380" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5381">
@@ -27365,7 +27365,7 @@
     </row>
     <row r="5387">
       <c r="A5387" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5388">
@@ -28450,7 +28450,7 @@
     </row>
     <row r="5604">
       <c r="A5604" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5605">
@@ -28540,7 +28540,7 @@
     </row>
     <row r="5622">
       <c r="A5622" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5623">
@@ -29795,7 +29795,7 @@
     </row>
     <row r="5873">
       <c r="A5873" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5874">
@@ -30395,7 +30395,7 @@
     </row>
     <row r="5993">
       <c r="A5993" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5994">
@@ -32855,7 +32855,7 @@
     </row>
     <row r="6485">
       <c r="A6485" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6486">
@@ -32960,7 +32960,7 @@
     </row>
     <row r="6506">
       <c r="A6506" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6507">
@@ -33900,7 +33900,7 @@
     </row>
     <row r="6694">
       <c r="A6694" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6695">
@@ -35670,7 +35670,7 @@
     </row>
     <row r="7048">
       <c r="A7048" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7049">
@@ -36300,7 +36300,7 @@
     </row>
     <row r="7174">
       <c r="A7174" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7175">
@@ -38085,7 +38085,7 @@
     </row>
     <row r="7531">
       <c r="A7531" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7532">
@@ -38525,7 +38525,7 @@
     </row>
     <row r="7619">
       <c r="A7619" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7620">
@@ -38675,7 +38675,7 @@
     </row>
     <row r="7649">
       <c r="A7649" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7650">
@@ -40205,7 +40205,7 @@
     </row>
     <row r="7955">
       <c r="A7955" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7956">
@@ -41310,7 +41310,7 @@
     </row>
     <row r="8176">
       <c r="A8176" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8177">
@@ -41610,7 +41610,7 @@
     </row>
     <row r="8236">
       <c r="A8236" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8237">
@@ -41905,7 +41905,7 @@
     </row>
     <row r="8295">
       <c r="A8295" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8296">
@@ -42245,7 +42245,7 @@
     </row>
     <row r="8363">
       <c r="A8363" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8364">
@@ -42560,7 +42560,7 @@
     </row>
     <row r="8426">
       <c r="A8426" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8427">
@@ -42605,7 +42605,7 @@
     </row>
     <row r="8435">
       <c r="A8435" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8436">

</xml_diff>